<commit_message>
correcion de valor renominado
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaReporteDiario.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaReporteDiario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppV2\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1807EF67-44D4-47BF-BC8F-61E136966B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B67D0F-740E-4A9E-BC46-1B81CE707D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="664" xr2:uid="{3B2FCDE3-AFC0-46E3-A7F2-136C8F41A25F}"/>
   </bookViews>
@@ -1519,22 +1519,28 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1549,97 +1555,28 @@
     <xf numFmtId="164" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1675,16 +1612,79 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -30699,8 +30699,8 @@
   </sheetPr>
   <dimension ref="A1:X285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -30736,63 +30736,63 @@
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="152" t="s">
+      <c r="E1" s="131" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
-      <c r="H1" s="152"/>
-      <c r="I1" s="152"/>
-      <c r="J1" s="152"/>
-      <c r="K1" s="152"/>
-      <c r="L1" s="155" t="s">
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="134" t="s">
         <v>154</v>
       </c>
-      <c r="M1" s="156"/>
+      <c r="M1" s="135"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5"/>
       <c r="C2" s="28"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="157" t="s">
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="158"/>
+      <c r="M2" s="137"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="28"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="153"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
-      <c r="J3" s="153"/>
-      <c r="K3" s="153"/>
-      <c r="L3" s="159" t="s">
+      <c r="E3" s="132"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="138" t="s">
         <v>153</v>
       </c>
-      <c r="M3" s="160"/>
+      <c r="M3" s="139"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="28"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
-      <c r="J4" s="153"/>
-      <c r="K4" s="153"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
+      <c r="H4" s="132"/>
+      <c r="I4" s="132"/>
+      <c r="J4" s="132"/>
+      <c r="K4" s="132"/>
       <c r="L4" s="53" t="s">
         <v>7</v>
       </c>
@@ -30804,13 +30804,13 @@
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="154"/>
-      <c r="G5" s="154"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
-      <c r="K5" s="154"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="133"/>
       <c r="L5" s="87" t="s">
         <v>155</v>
       </c>
@@ -30872,54 +30872,54 @@
     <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="60"/>
       <c r="B11" s="75"/>
-      <c r="C11" s="146" t="s">
+      <c r="C11" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="146"/>
-      <c r="E11" s="146"/>
-      <c r="F11" s="146"/>
-      <c r="G11" s="146"/>
-      <c r="H11" s="146"/>
-      <c r="I11" s="146"/>
-      <c r="J11" s="146"/>
-      <c r="K11" s="146"/>
-      <c r="L11" s="146"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="118"/>
+      <c r="J11" s="118"/>
+      <c r="K11" s="118"/>
+      <c r="L11" s="118"/>
       <c r="M11" s="82"/>
     </row>
     <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="60"/>
       <c r="B12" s="75"/>
-      <c r="C12" s="146"/>
-      <c r="D12" s="146"/>
-      <c r="E12" s="146"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="146"/>
-      <c r="K12" s="146"/>
-      <c r="L12" s="146"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="118"/>
+      <c r="L12" s="118"/>
       <c r="M12" s="82"/>
     </row>
     <row r="13" spans="1:16" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="60"/>
       <c r="B13" s="75"/>
-      <c r="C13" s="146" t="s">
+      <c r="C13" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="146"/>
+      <c r="D13" s="118"/>
       <c r="E13" s="68" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="146" t="s">
+      <c r="G13" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="146"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="146"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
+      <c r="J13" s="118"/>
       <c r="K13" s="68" t="s">
         <v>15</v>
       </c>
@@ -30931,22 +30931,22 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="60"/>
       <c r="B14" s="75"/>
-      <c r="C14" s="146"/>
-      <c r="D14" s="146"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
       <c r="E14" s="67" t="s">
         <v>45</v>
       </c>
       <c r="F14" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="161" t="s">
+      <c r="G14" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="161"/>
-      <c r="I14" s="161" t="s">
+      <c r="H14" s="140"/>
+      <c r="I14" s="140" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="161"/>
+      <c r="J14" s="140"/>
       <c r="K14" s="67" t="s">
         <v>16</v>
       </c>
@@ -30958,24 +30958,24 @@
     <row r="15" spans="1:16" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="60"/>
       <c r="B15" s="75"/>
-      <c r="C15" s="164" t="s">
+      <c r="C15" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="164"/>
+      <c r="D15" s="113"/>
       <c r="E15" s="101" t="s">
         <v>72</v>
       </c>
       <c r="F15" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="162" t="s">
+      <c r="G15" s="141" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="162"/>
-      <c r="I15" s="133" t="s">
+      <c r="H15" s="141"/>
+      <c r="I15" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="J15" s="133"/>
+      <c r="J15" s="142"/>
       <c r="K15" s="100" t="s">
         <v>74</v>
       </c>
@@ -30987,14 +30987,14 @@
     <row r="16" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="60"/>
       <c r="B16" s="75"/>
-      <c r="C16" s="164"/>
-      <c r="D16" s="164"/>
+      <c r="C16" s="113"/>
+      <c r="D16" s="113"/>
       <c r="E16" s="95"/>
       <c r="F16" s="95"/>
-      <c r="G16" s="162"/>
-      <c r="H16" s="162"/>
-      <c r="I16" s="133"/>
-      <c r="J16" s="133"/>
+      <c r="G16" s="141"/>
+      <c r="H16" s="141"/>
+      <c r="I16" s="142"/>
+      <c r="J16" s="142"/>
       <c r="K16" s="100"/>
       <c r="L16" s="100"/>
       <c r="M16" s="83"/>
@@ -31014,18 +31014,18 @@
     <row r="18" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="60"/>
       <c r="B18" s="75"/>
-      <c r="C18" s="132" t="s">
+      <c r="C18" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="132"/>
-      <c r="E18" s="132"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
       <c r="F18" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="134" t="s">
+      <c r="H18" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="I18" s="134"/>
+      <c r="I18" s="117"/>
       <c r="J18" s="69" t="s">
         <v>76</v>
       </c>
@@ -31037,11 +31037,11 @@
     <row r="19" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="60"/>
       <c r="B19" s="75"/>
-      <c r="C19" s="132" t="s">
+      <c r="C19" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="132"/>
-      <c r="E19" s="132"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
       <c r="F19" s="58" t="s">
         <v>68</v>
       </c>
@@ -31056,11 +31056,11 @@
     <row r="20" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="60"/>
       <c r="B20" s="75"/>
-      <c r="C20" s="147" t="s">
+      <c r="C20" s="153" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="147"/>
-      <c r="E20" s="147"/>
+      <c r="D20" s="153"/>
+      <c r="E20" s="153"/>
       <c r="F20" s="106" t="s">
         <v>69</v>
       </c>
@@ -31129,158 +31129,158 @@
     <row r="25" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="60"/>
       <c r="B25" s="75"/>
-      <c r="C25" s="146" t="s">
+      <c r="C25" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="146"/>
-      <c r="E25" s="146"/>
-      <c r="F25" s="146"/>
-      <c r="G25" s="146"/>
-      <c r="H25" s="146"/>
-      <c r="I25" s="146"/>
-      <c r="J25" s="146"/>
-      <c r="K25" s="146"/>
-      <c r="L25" s="146"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="118"/>
+      <c r="G25" s="118"/>
+      <c r="H25" s="118"/>
+      <c r="I25" s="118"/>
+      <c r="J25" s="118"/>
+      <c r="K25" s="118"/>
+      <c r="L25" s="118"/>
       <c r="M25" s="81"/>
       <c r="P25" s="13"/>
     </row>
     <row r="26" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="60"/>
       <c r="B26" s="75"/>
-      <c r="C26" s="146"/>
-      <c r="D26" s="146"/>
-      <c r="E26" s="146"/>
-      <c r="F26" s="146"/>
-      <c r="G26" s="146"/>
-      <c r="H26" s="146"/>
-      <c r="I26" s="146"/>
-      <c r="J26" s="146"/>
-      <c r="K26" s="146"/>
-      <c r="L26" s="146"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="118"/>
+      <c r="F26" s="118"/>
+      <c r="G26" s="118"/>
+      <c r="H26" s="118"/>
+      <c r="I26" s="118"/>
+      <c r="J26" s="118"/>
+      <c r="K26" s="118"/>
+      <c r="L26" s="118"/>
       <c r="M26" s="81"/>
       <c r="P26" s="13"/>
     </row>
     <row r="27" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="60"/>
       <c r="B27" s="75"/>
-      <c r="C27" s="146"/>
-      <c r="D27" s="146"/>
-      <c r="E27" s="146"/>
-      <c r="F27" s="146"/>
-      <c r="G27" s="146"/>
-      <c r="H27" s="146"/>
-      <c r="I27" s="146"/>
-      <c r="J27" s="146"/>
-      <c r="K27" s="146"/>
-      <c r="L27" s="146"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="118"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="118"/>
+      <c r="H27" s="118"/>
+      <c r="I27" s="118"/>
+      <c r="J27" s="118"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="118"/>
       <c r="M27" s="81"/>
       <c r="P27" s="13"/>
     </row>
     <row r="28" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="60"/>
       <c r="B28" s="75"/>
-      <c r="C28" s="126" t="s">
+      <c r="C28" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="126"/>
-      <c r="E28" s="113" t="s">
+      <c r="D28" s="125"/>
+      <c r="E28" s="127" t="s">
         <v>159</v>
       </c>
-      <c r="F28" s="114"/>
-      <c r="G28" s="113" t="s">
+      <c r="F28" s="128"/>
+      <c r="G28" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="114"/>
-      <c r="I28" s="117" t="s">
+      <c r="H28" s="128"/>
+      <c r="I28" s="119" t="s">
         <v>65</v>
       </c>
-      <c r="J28" s="123"/>
-      <c r="K28" s="126" t="s">
+      <c r="J28" s="158"/>
+      <c r="K28" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="L28" s="126"/>
+      <c r="L28" s="125"/>
       <c r="M28" s="81"/>
       <c r="P28" s="13"/>
     </row>
     <row r="29" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="60"/>
       <c r="B29" s="75"/>
-      <c r="C29" s="126"/>
-      <c r="D29" s="126"/>
-      <c r="E29" s="115"/>
-      <c r="F29" s="116"/>
-      <c r="G29" s="115"/>
-      <c r="H29" s="116"/>
-      <c r="I29" s="119"/>
-      <c r="J29" s="124"/>
-      <c r="K29" s="126"/>
-      <c r="L29" s="126"/>
+      <c r="C29" s="125"/>
+      <c r="D29" s="125"/>
+      <c r="E29" s="129"/>
+      <c r="F29" s="130"/>
+      <c r="G29" s="129"/>
+      <c r="H29" s="130"/>
+      <c r="I29" s="121"/>
+      <c r="J29" s="159"/>
+      <c r="K29" s="125"/>
+      <c r="L29" s="125"/>
       <c r="M29" s="81"/>
       <c r="P29" s="13"/>
     </row>
     <row r="30" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="60"/>
       <c r="B30" s="75"/>
-      <c r="C30" s="126"/>
-      <c r="D30" s="126"/>
-      <c r="E30" s="166" t="s">
+      <c r="C30" s="125"/>
+      <c r="D30" s="125"/>
+      <c r="E30" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="126"/>
-      <c r="G30" s="126" t="s">
+      <c r="F30" s="125"/>
+      <c r="G30" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="126"/>
-      <c r="I30" s="126" t="s">
+      <c r="H30" s="125"/>
+      <c r="I30" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="J30" s="126"/>
-      <c r="K30" s="143" t="s">
+      <c r="J30" s="125"/>
+      <c r="K30" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="L30" s="143"/>
+      <c r="L30" s="148"/>
       <c r="M30" s="81"/>
       <c r="P30" s="13"/>
     </row>
     <row r="31" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="60"/>
       <c r="B31" s="75"/>
-      <c r="C31" s="142" t="s">
+      <c r="C31" s="152" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="142"/>
-      <c r="E31" s="144" t="s">
+      <c r="D31" s="152"/>
+      <c r="E31" s="142" t="s">
         <v>72</v>
       </c>
-      <c r="F31" s="144"/>
-      <c r="G31" s="133" t="s">
+      <c r="F31" s="142"/>
+      <c r="G31" s="142" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="133"/>
-      <c r="I31" s="144" t="s">
+      <c r="H31" s="142"/>
+      <c r="I31" s="151" t="s">
         <v>75</v>
       </c>
-      <c r="J31" s="144"/>
-      <c r="K31" s="133" t="s">
+      <c r="J31" s="151"/>
+      <c r="K31" s="142" t="s">
         <v>74</v>
       </c>
-      <c r="L31" s="133"/>
+      <c r="L31" s="142"/>
       <c r="M31" s="81"/>
       <c r="P31" s="13"/>
     </row>
     <row r="32" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="60"/>
       <c r="B32" s="75"/>
-      <c r="C32" s="142"/>
-      <c r="D32" s="142"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="133"/>
-      <c r="H32" s="133"/>
-      <c r="I32" s="144"/>
-      <c r="J32" s="144"/>
-      <c r="K32" s="133"/>
-      <c r="L32" s="133"/>
+      <c r="C32" s="152"/>
+      <c r="D32" s="152"/>
+      <c r="E32" s="142"/>
+      <c r="F32" s="142"/>
+      <c r="G32" s="142"/>
+      <c r="H32" s="142"/>
+      <c r="I32" s="151"/>
+      <c r="J32" s="151"/>
+      <c r="K32" s="142"/>
+      <c r="L32" s="142"/>
       <c r="M32" s="81"/>
       <c r="P32" s="13"/>
     </row>
@@ -31337,10 +31337,10 @@
     <row r="37" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="60"/>
       <c r="B37" s="75"/>
-      <c r="C37" s="165" t="s">
+      <c r="C37" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="165"/>
+      <c r="D37" s="114"/>
       <c r="E37" s="103" t="s">
         <v>70</v>
       </c>
@@ -31364,34 +31364,34 @@
     <row r="39" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="60"/>
       <c r="B39" s="75"/>
-      <c r="C39" s="126" t="s">
+      <c r="C39" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="126"/>
-      <c r="E39" s="126"/>
-      <c r="F39" s="126"/>
-      <c r="G39" s="126"/>
-      <c r="H39" s="126"/>
-      <c r="I39" s="146" t="s">
+      <c r="D39" s="125"/>
+      <c r="E39" s="125"/>
+      <c r="F39" s="125"/>
+      <c r="G39" s="125"/>
+      <c r="H39" s="125"/>
+      <c r="I39" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="J39" s="146"/>
-      <c r="K39" s="146" t="s">
+      <c r="J39" s="118"/>
+      <c r="K39" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="L39" s="146"/>
+      <c r="L39" s="118"/>
       <c r="M39" s="81"/>
       <c r="P39" s="13"/>
     </row>
     <row r="40" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="60"/>
       <c r="B40" s="75"/>
-      <c r="C40" s="126"/>
-      <c r="D40" s="126"/>
-      <c r="E40" s="126"/>
-      <c r="F40" s="126"/>
-      <c r="G40" s="126"/>
-      <c r="H40" s="126"/>
+      <c r="C40" s="125"/>
+      <c r="D40" s="125"/>
+      <c r="E40" s="125"/>
+      <c r="F40" s="125"/>
+      <c r="G40" s="125"/>
+      <c r="H40" s="125"/>
       <c r="I40" s="16" t="s">
         <v>27</v>
       </c>
@@ -31410,12 +31410,12 @@
     <row r="41" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="60"/>
       <c r="B41" s="75"/>
-      <c r="C41" s="126"/>
-      <c r="D41" s="126"/>
-      <c r="E41" s="126"/>
-      <c r="F41" s="126"/>
-      <c r="G41" s="126"/>
-      <c r="H41" s="126"/>
+      <c r="C41" s="125"/>
+      <c r="D41" s="125"/>
+      <c r="E41" s="125"/>
+      <c r="F41" s="125"/>
+      <c r="G41" s="125"/>
+      <c r="H41" s="125"/>
       <c r="I41" s="56" t="s">
         <v>30</v>
       </c>
@@ -31441,14 +31441,14 @@
     <row r="42" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="60"/>
       <c r="B42" s="75"/>
-      <c r="C42" s="138" t="s">
+      <c r="C42" s="116" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="138"/>
-      <c r="E42" s="138"/>
-      <c r="F42" s="138"/>
-      <c r="G42" s="138"/>
-      <c r="H42" s="138"/>
+      <c r="D42" s="116"/>
+      <c r="E42" s="116"/>
+      <c r="F42" s="116"/>
+      <c r="G42" s="116"/>
+      <c r="H42" s="116"/>
       <c r="I42" s="99" t="s">
         <v>79</v>
       </c>
@@ -31466,12 +31466,12 @@
     <row r="43" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="60"/>
       <c r="B43" s="75"/>
-      <c r="C43" s="138"/>
-      <c r="D43" s="138"/>
-      <c r="E43" s="138"/>
-      <c r="F43" s="138"/>
-      <c r="G43" s="138"/>
-      <c r="H43" s="138"/>
+      <c r="C43" s="116"/>
+      <c r="D43" s="116"/>
+      <c r="E43" s="116"/>
+      <c r="F43" s="116"/>
+      <c r="G43" s="116"/>
+      <c r="H43" s="116"/>
       <c r="I43" s="99"/>
       <c r="J43" s="99"/>
       <c r="K43" s="99"/>
@@ -31491,18 +31491,18 @@
     <row r="46" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="60"/>
       <c r="B46" s="75"/>
-      <c r="C46" s="145" t="s">
+      <c r="C46" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="138"/>
-      <c r="E46" s="138"/>
-      <c r="F46" s="138"/>
-      <c r="G46" s="138"/>
-      <c r="H46" s="138"/>
-      <c r="I46" s="138"/>
-      <c r="J46" s="138"/>
-      <c r="K46" s="138"/>
-      <c r="L46" s="138"/>
+      <c r="D46" s="116"/>
+      <c r="E46" s="116"/>
+      <c r="F46" s="116"/>
+      <c r="G46" s="116"/>
+      <c r="H46" s="116"/>
+      <c r="I46" s="116"/>
+      <c r="J46" s="116"/>
+      <c r="K46" s="116"/>
+      <c r="L46" s="116"/>
       <c r="M46" s="84"/>
       <c r="N46" s="21"/>
       <c r="P46" s="13"/>
@@ -31660,18 +31660,18 @@
     <row r="52" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="60"/>
       <c r="B52" s="75"/>
-      <c r="C52" s="145" t="s">
+      <c r="C52" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="D52" s="138"/>
-      <c r="E52" s="138"/>
-      <c r="F52" s="138"/>
-      <c r="G52" s="138"/>
-      <c r="H52" s="138"/>
-      <c r="I52" s="138"/>
-      <c r="J52" s="138"/>
-      <c r="K52" s="138"/>
-      <c r="L52" s="138"/>
+      <c r="D52" s="116"/>
+      <c r="E52" s="116"/>
+      <c r="F52" s="116"/>
+      <c r="G52" s="116"/>
+      <c r="H52" s="116"/>
+      <c r="I52" s="116"/>
+      <c r="J52" s="116"/>
+      <c r="K52" s="116"/>
+      <c r="L52" s="116"/>
       <c r="M52" s="81"/>
       <c r="P52" s="13"/>
       <c r="R52" s="17"/>
@@ -31857,49 +31857,49 @@
     <row r="61" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="60"/>
       <c r="B61" s="10"/>
-      <c r="C61" s="146" t="s">
+      <c r="C61" s="118" t="s">
         <v>161</v>
       </c>
-      <c r="D61" s="146"/>
-      <c r="E61" s="146"/>
+      <c r="D61" s="118"/>
+      <c r="E61" s="118"/>
       <c r="F61" s="34"/>
-      <c r="H61" s="117" t="s">
+      <c r="H61" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="I61" s="123"/>
-      <c r="J61" s="118"/>
+      <c r="I61" s="158"/>
+      <c r="J61" s="120"/>
       <c r="M61" s="83"/>
       <c r="N61" s="20"/>
     </row>
     <row r="62" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="60"/>
       <c r="B62" s="10"/>
-      <c r="C62" s="113" t="s">
+      <c r="C62" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="D62" s="114"/>
-      <c r="E62" s="111" t="s">
+      <c r="D62" s="128"/>
+      <c r="E62" s="123" t="s">
         <v>13</v>
       </c>
       <c r="F62" s="34"/>
-      <c r="H62" s="119"/>
-      <c r="I62" s="124"/>
-      <c r="J62" s="120"/>
+      <c r="H62" s="121"/>
+      <c r="I62" s="159"/>
+      <c r="J62" s="122"/>
       <c r="M62" s="83"/>
       <c r="N62" s="20"/>
     </row>
     <row r="63" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="60"/>
       <c r="B63" s="10"/>
-      <c r="C63" s="139"/>
-      <c r="D63" s="140"/>
-      <c r="E63" s="141"/>
+      <c r="C63" s="155"/>
+      <c r="D63" s="156"/>
+      <c r="E63" s="157"/>
       <c r="F63" s="34"/>
-      <c r="H63" s="117" t="s">
+      <c r="H63" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="I63" s="118"/>
-      <c r="J63" s="111" t="s">
+      <c r="I63" s="120"/>
+      <c r="J63" s="123" t="s">
         <v>56</v>
       </c>
       <c r="M63" s="83"/>
@@ -31908,33 +31908,33 @@
     <row r="64" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="60"/>
       <c r="B64" s="10"/>
-      <c r="C64" s="115"/>
-      <c r="D64" s="116"/>
+      <c r="C64" s="129"/>
+      <c r="D64" s="130"/>
       <c r="E64" s="109" t="s">
         <v>45</v>
       </c>
       <c r="F64" s="34"/>
-      <c r="H64" s="119"/>
-      <c r="I64" s="120"/>
-      <c r="J64" s="112"/>
+      <c r="H64" s="121"/>
+      <c r="I64" s="122"/>
+      <c r="J64" s="124"/>
       <c r="M64" s="83"/>
       <c r="N64" s="20"/>
     </row>
     <row r="65" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="60"/>
       <c r="B65" s="10"/>
-      <c r="C65" s="134" t="s">
+      <c r="C65" s="117" t="s">
         <v>97</v>
       </c>
-      <c r="D65" s="134"/>
+      <c r="D65" s="117"/>
       <c r="E65" s="105" t="s">
         <v>102</v>
       </c>
       <c r="F65" s="34"/>
-      <c r="H65" s="135" t="s">
+      <c r="H65" s="149" t="s">
         <v>99</v>
       </c>
-      <c r="I65" s="136"/>
+      <c r="I65" s="150"/>
       <c r="J65" s="104" t="s">
         <v>104</v>
       </c>
@@ -31944,18 +31944,18 @@
     <row r="66" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="60"/>
       <c r="B66" s="10"/>
-      <c r="C66" s="134" t="s">
+      <c r="C66" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="D66" s="134"/>
+      <c r="D66" s="117"/>
       <c r="E66" s="105" t="s">
         <v>103</v>
       </c>
       <c r="F66" s="34"/>
-      <c r="H66" s="135" t="s">
+      <c r="H66" s="149" t="s">
         <v>100</v>
       </c>
-      <c r="I66" s="136"/>
+      <c r="I66" s="150"/>
       <c r="J66" s="104" t="s">
         <v>105</v>
       </c>
@@ -31968,10 +31968,10 @@
       <c r="C67" s="29"/>
       <c r="E67" s="34"/>
       <c r="F67" s="34"/>
-      <c r="H67" s="137" t="s">
+      <c r="H67" s="154" t="s">
         <v>101</v>
       </c>
-      <c r="I67" s="137"/>
+      <c r="I67" s="154"/>
       <c r="J67" s="110" t="s">
         <v>106</v>
       </c>
@@ -32021,52 +32021,52 @@
     <row r="72" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="60"/>
       <c r="B72" s="10"/>
-      <c r="C72" s="113" t="s">
+      <c r="C72" s="127" t="s">
         <v>50</v>
       </c>
-      <c r="D72" s="121"/>
-      <c r="E72" s="114"/>
+      <c r="D72" s="161"/>
+      <c r="E72" s="128"/>
       <c r="F72" s="12"/>
       <c r="G72" s="12"/>
-      <c r="H72" s="117" t="s">
+      <c r="H72" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="I72" s="123"/>
-      <c r="J72" s="118"/>
+      <c r="I72" s="158"/>
+      <c r="J72" s="120"/>
       <c r="M72" s="83"/>
       <c r="N72" s="20"/>
     </row>
     <row r="73" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="60"/>
       <c r="B73" s="10"/>
-      <c r="C73" s="115"/>
-      <c r="D73" s="122"/>
-      <c r="E73" s="116"/>
+      <c r="C73" s="129"/>
+      <c r="D73" s="162"/>
+      <c r="E73" s="130"/>
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
-      <c r="H73" s="119"/>
-      <c r="I73" s="124"/>
-      <c r="J73" s="120"/>
+      <c r="H73" s="121"/>
+      <c r="I73" s="159"/>
+      <c r="J73" s="122"/>
       <c r="M73" s="83"/>
       <c r="N73" s="20"/>
     </row>
     <row r="74" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="60"/>
       <c r="B74" s="10"/>
-      <c r="C74" s="113" t="s">
+      <c r="C74" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="D74" s="114"/>
-      <c r="E74" s="111" t="s">
+      <c r="D74" s="128"/>
+      <c r="E74" s="123" t="s">
         <v>52</v>
       </c>
       <c r="F74" s="12"/>
       <c r="G74" s="12"/>
-      <c r="H74" s="117" t="s">
+      <c r="H74" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="I74" s="118"/>
-      <c r="J74" s="111" t="s">
+      <c r="I74" s="120"/>
+      <c r="J74" s="123" t="s">
         <v>56</v>
       </c>
       <c r="M74" s="83"/>
@@ -32075,32 +32075,32 @@
     <row r="75" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="60"/>
       <c r="B75" s="10"/>
-      <c r="C75" s="115"/>
-      <c r="D75" s="116"/>
-      <c r="E75" s="112"/>
+      <c r="C75" s="129"/>
+      <c r="D75" s="130"/>
+      <c r="E75" s="124"/>
       <c r="F75" s="12"/>
       <c r="G75" s="12"/>
-      <c r="H75" s="119"/>
-      <c r="I75" s="120"/>
-      <c r="J75" s="112"/>
+      <c r="H75" s="121"/>
+      <c r="I75" s="122"/>
+      <c r="J75" s="124"/>
       <c r="M75" s="83"/>
       <c r="N75" s="20"/>
     </row>
     <row r="76" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="60"/>
       <c r="B76" s="75"/>
-      <c r="C76" s="132" t="s">
+      <c r="C76" s="112" t="s">
         <v>110</v>
       </c>
-      <c r="D76" s="132"/>
+      <c r="D76" s="112"/>
       <c r="E76" s="108" t="s">
         <v>114</v>
       </c>
       <c r="F76" s="22"/>
-      <c r="H76" s="137" t="s">
+      <c r="H76" s="154" t="s">
         <v>99</v>
       </c>
-      <c r="I76" s="137"/>
+      <c r="I76" s="154"/>
       <c r="J76" s="104" t="s">
         <v>107</v>
       </c>
@@ -32112,18 +32112,18 @@
     <row r="77" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="60"/>
       <c r="B77" s="75"/>
-      <c r="C77" s="132" t="s">
+      <c r="C77" s="112" t="s">
         <v>111</v>
       </c>
-      <c r="D77" s="132"/>
+      <c r="D77" s="112"/>
       <c r="E77" s="108" t="s">
         <v>115</v>
       </c>
       <c r="F77" s="22"/>
-      <c r="H77" s="137" t="s">
+      <c r="H77" s="154" t="s">
         <v>100</v>
       </c>
-      <c r="I77" s="137"/>
+      <c r="I77" s="154"/>
       <c r="J77" s="104" t="s">
         <v>108</v>
       </c>
@@ -32135,18 +32135,18 @@
     <row r="78" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="60"/>
       <c r="B78" s="75"/>
-      <c r="C78" s="132" t="s">
+      <c r="C78" s="112" t="s">
         <v>112</v>
       </c>
-      <c r="D78" s="132"/>
+      <c r="D78" s="112"/>
       <c r="E78" s="108" t="s">
         <v>116</v>
       </c>
       <c r="F78" s="22"/>
-      <c r="H78" s="137" t="s">
+      <c r="H78" s="154" t="s">
         <v>101</v>
       </c>
-      <c r="I78" s="137"/>
+      <c r="I78" s="154"/>
       <c r="J78" s="104" t="s">
         <v>109</v>
       </c>
@@ -32158,10 +32158,10 @@
     <row r="79" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="60"/>
       <c r="B79" s="75"/>
-      <c r="C79" s="132" t="s">
+      <c r="C79" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="D79" s="132"/>
+      <c r="D79" s="112"/>
       <c r="E79" s="108" t="s">
         <v>117</v>
       </c>
@@ -32174,10 +32174,10 @@
     <row r="80" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="60"/>
       <c r="B80" s="75"/>
-      <c r="C80" s="132" t="s">
+      <c r="C80" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="D80" s="132"/>
+      <c r="D80" s="112"/>
       <c r="E80" s="108" t="s">
         <v>118</v>
       </c>
@@ -32251,19 +32251,19 @@
     <row r="86" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="60"/>
       <c r="B86" s="75"/>
-      <c r="C86" s="146" t="s">
+      <c r="C86" s="118" t="s">
         <v>48</v>
       </c>
-      <c r="D86" s="146"/>
-      <c r="E86" s="146"/>
-      <c r="F86" s="146"/>
+      <c r="D86" s="118"/>
+      <c r="E86" s="118"/>
+      <c r="F86" s="118"/>
       <c r="G86" s="12"/>
-      <c r="H86" s="148" t="s">
+      <c r="H86" s="144" t="s">
         <v>55</v>
       </c>
-      <c r="I86" s="148"/>
-      <c r="J86" s="148"/>
-      <c r="K86" s="148"/>
+      <c r="I86" s="144"/>
+      <c r="J86" s="144"/>
+      <c r="K86" s="144"/>
       <c r="L86" s="33"/>
       <c r="M86" s="81"/>
       <c r="N86" s="20"/>
@@ -32272,14 +32272,14 @@
     <row r="87" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="60"/>
       <c r="B87" s="75"/>
-      <c r="C87" s="113" t="s">
+      <c r="C87" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="D87" s="114"/>
-      <c r="E87" s="111" t="s">
+      <c r="D87" s="128"/>
+      <c r="E87" s="123" t="s">
         <v>47</v>
       </c>
-      <c r="F87" s="111" t="s">
+      <c r="F87" s="123" t="s">
         <v>43</v>
       </c>
       <c r="H87" s="63" t="s">
@@ -32301,10 +32301,10 @@
     <row r="88" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="60"/>
       <c r="B88" s="75"/>
-      <c r="C88" s="115"/>
-      <c r="D88" s="116"/>
-      <c r="E88" s="112"/>
-      <c r="F88" s="112"/>
+      <c r="C88" s="129"/>
+      <c r="D88" s="130"/>
+      <c r="E88" s="124"/>
+      <c r="F88" s="124"/>
       <c r="H88" s="64" t="s">
         <v>99</v>
       </c>
@@ -32324,10 +32324,10 @@
     <row r="89" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="60"/>
       <c r="B89" s="75"/>
-      <c r="C89" s="150" t="s">
+      <c r="C89" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="D89" s="151"/>
+      <c r="D89" s="147"/>
       <c r="E89" s="96" t="s">
         <v>119</v>
       </c>
@@ -32353,10 +32353,10 @@
     <row r="90" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="60"/>
       <c r="B90" s="75"/>
-      <c r="C90" s="150" t="s">
+      <c r="C90" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="D90" s="151"/>
+      <c r="D90" s="147"/>
       <c r="E90" s="96" t="s">
         <v>120</v>
       </c>
@@ -32382,10 +32382,10 @@
     <row r="91" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="60"/>
       <c r="B91" s="75"/>
-      <c r="C91" s="150" t="s">
+      <c r="C91" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="D91" s="151"/>
+      <c r="D91" s="147"/>
       <c r="E91" s="96" t="s">
         <v>121</v>
       </c>
@@ -32399,10 +32399,10 @@
     <row r="92" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="60"/>
       <c r="B92" s="75"/>
-      <c r="C92" s="150" t="s">
+      <c r="C92" s="146" t="s">
         <v>101</v>
       </c>
-      <c r="D92" s="151"/>
+      <c r="D92" s="147"/>
       <c r="E92" s="96" t="s">
         <v>122</v>
       </c>
@@ -32430,11 +32430,11 @@
     <row r="94" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="60"/>
       <c r="B94" s="75"/>
-      <c r="C94" s="149" t="s">
+      <c r="C94" s="145" t="s">
         <v>44</v>
       </c>
-      <c r="D94" s="149"/>
-      <c r="E94" s="149"/>
+      <c r="D94" s="145"/>
+      <c r="E94" s="145"/>
       <c r="F94" s="98" t="s">
         <v>135</v>
       </c>
@@ -32477,17 +32477,17 @@
     <row r="98" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="60"/>
       <c r="B98" s="75"/>
-      <c r="C98" s="113" t="s">
+      <c r="C98" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="D98" s="121"/>
-      <c r="E98" s="114"/>
+      <c r="D98" s="161"/>
+      <c r="E98" s="128"/>
       <c r="F98" s="12"/>
       <c r="G98" s="12"/>
-      <c r="H98" s="117" t="s">
+      <c r="H98" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="I98" s="118"/>
+      <c r="I98" s="120"/>
       <c r="L98" s="33"/>
       <c r="M98" s="81"/>
       <c r="N98" s="20"/>
@@ -32496,13 +32496,13 @@
     <row r="99" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="60"/>
       <c r="B99" s="75"/>
-      <c r="C99" s="115"/>
-      <c r="D99" s="122"/>
-      <c r="E99" s="116"/>
+      <c r="C99" s="129"/>
+      <c r="D99" s="162"/>
+      <c r="E99" s="130"/>
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
-      <c r="H99" s="119"/>
-      <c r="I99" s="120"/>
+      <c r="H99" s="121"/>
+      <c r="I99" s="122"/>
       <c r="L99" s="33"/>
       <c r="M99" s="81"/>
       <c r="N99" s="20"/>
@@ -32511,19 +32511,19 @@
     <row r="100" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="60"/>
       <c r="B100" s="75"/>
-      <c r="C100" s="113" t="s">
+      <c r="C100" s="127" t="s">
         <v>51</v>
       </c>
-      <c r="D100" s="114"/>
-      <c r="E100" s="111" t="s">
+      <c r="D100" s="128"/>
+      <c r="E100" s="123" t="s">
         <v>52</v>
       </c>
       <c r="F100" s="12"/>
       <c r="G100" s="12"/>
-      <c r="H100" s="127" t="s">
+      <c r="H100" s="163" t="s">
         <v>53</v>
       </c>
-      <c r="I100" s="129" t="s">
+      <c r="I100" s="165" t="s">
         <v>56</v>
       </c>
       <c r="L100" s="33"/>
@@ -32534,12 +32534,12 @@
     <row r="101" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="60"/>
       <c r="B101" s="75"/>
-      <c r="C101" s="115"/>
-      <c r="D101" s="116"/>
-      <c r="E101" s="112"/>
+      <c r="C101" s="129"/>
+      <c r="D101" s="130"/>
+      <c r="E101" s="124"/>
       <c r="F101" s="22"/>
-      <c r="H101" s="128"/>
-      <c r="I101" s="130"/>
+      <c r="H101" s="164"/>
+      <c r="I101" s="166"/>
       <c r="J101" s="14"/>
       <c r="K101" s="14"/>
       <c r="L101" s="33"/>
@@ -32549,10 +32549,10 @@
     <row r="102" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="60"/>
       <c r="B102" s="75"/>
-      <c r="C102" s="131" t="s">
+      <c r="C102" s="143" t="s">
         <v>136</v>
       </c>
-      <c r="D102" s="131"/>
+      <c r="D102" s="143"/>
       <c r="E102" s="107" t="s">
         <v>142</v>
       </c>
@@ -32568,10 +32568,10 @@
     <row r="103" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="60"/>
       <c r="B103" s="75"/>
-      <c r="C103" s="131" t="s">
+      <c r="C103" s="143" t="s">
         <v>137</v>
       </c>
-      <c r="D103" s="131"/>
+      <c r="D103" s="143"/>
       <c r="E103" s="107" t="s">
         <v>143</v>
       </c>
@@ -32587,10 +32587,10 @@
     <row r="104" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="60"/>
       <c r="B104" s="75"/>
-      <c r="C104" s="131" t="s">
+      <c r="C104" s="143" t="s">
         <v>138</v>
       </c>
-      <c r="D104" s="131"/>
+      <c r="D104" s="143"/>
       <c r="E104" s="107" t="s">
         <v>144</v>
       </c>
@@ -32606,10 +32606,10 @@
     <row r="105" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="60"/>
       <c r="B105" s="75"/>
-      <c r="C105" s="131" t="s">
+      <c r="C105" s="143" t="s">
         <v>139</v>
       </c>
-      <c r="D105" s="131"/>
+      <c r="D105" s="143"/>
       <c r="E105" s="107" t="s">
         <v>145</v>
       </c>
@@ -32619,10 +32619,10 @@
     <row r="106" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="60"/>
       <c r="B106" s="75"/>
-      <c r="C106" s="131" t="s">
+      <c r="C106" s="143" t="s">
         <v>113</v>
       </c>
-      <c r="D106" s="131"/>
+      <c r="D106" s="143"/>
       <c r="E106" s="107" t="s">
         <v>146</v>
       </c>
@@ -32632,10 +32632,10 @@
     <row r="107" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="60"/>
       <c r="B107" s="75"/>
-      <c r="C107" s="131" t="s">
+      <c r="C107" s="143" t="s">
         <v>140</v>
       </c>
-      <c r="D107" s="131"/>
+      <c r="D107" s="143"/>
       <c r="E107" s="107" t="s">
         <v>147</v>
       </c>
@@ -32645,10 +32645,10 @@
     <row r="108" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="60"/>
       <c r="B108" s="75"/>
-      <c r="C108" s="131" t="s">
+      <c r="C108" s="143" t="s">
         <v>141</v>
       </c>
-      <c r="D108" s="131"/>
+      <c r="D108" s="143"/>
       <c r="E108" s="107" t="s">
         <v>148</v>
       </c>
@@ -32683,93 +32683,93 @@
     <row r="112" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="60"/>
       <c r="B112" s="76"/>
-      <c r="C112" s="125" t="s">
+      <c r="C112" s="160" t="s">
         <v>71</v>
       </c>
-      <c r="D112" s="125"/>
-      <c r="E112" s="125"/>
-      <c r="F112" s="125"/>
-      <c r="G112" s="125"/>
-      <c r="H112" s="125"/>
-      <c r="I112" s="125"/>
-      <c r="J112" s="125"/>
-      <c r="K112" s="125"/>
-      <c r="L112" s="125"/>
+      <c r="D112" s="160"/>
+      <c r="E112" s="160"/>
+      <c r="F112" s="160"/>
+      <c r="G112" s="160"/>
+      <c r="H112" s="160"/>
+      <c r="I112" s="160"/>
+      <c r="J112" s="160"/>
+      <c r="K112" s="160"/>
+      <c r="L112" s="160"/>
       <c r="M112" s="81"/>
     </row>
     <row r="113" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="60"/>
       <c r="B113" s="76"/>
-      <c r="C113" s="125"/>
-      <c r="D113" s="125"/>
-      <c r="E113" s="125"/>
-      <c r="F113" s="125"/>
-      <c r="G113" s="125"/>
-      <c r="H113" s="125"/>
-      <c r="I113" s="125"/>
-      <c r="J113" s="125"/>
-      <c r="K113" s="125"/>
-      <c r="L113" s="125"/>
+      <c r="C113" s="160"/>
+      <c r="D113" s="160"/>
+      <c r="E113" s="160"/>
+      <c r="F113" s="160"/>
+      <c r="G113" s="160"/>
+      <c r="H113" s="160"/>
+      <c r="I113" s="160"/>
+      <c r="J113" s="160"/>
+      <c r="K113" s="160"/>
+      <c r="L113" s="160"/>
       <c r="M113" s="81"/>
     </row>
     <row r="114" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="60"/>
       <c r="B114" s="76"/>
-      <c r="C114" s="125"/>
-      <c r="D114" s="125"/>
-      <c r="E114" s="125"/>
-      <c r="F114" s="125"/>
-      <c r="G114" s="125"/>
-      <c r="H114" s="125"/>
-      <c r="I114" s="125"/>
-      <c r="J114" s="125"/>
-      <c r="K114" s="125"/>
-      <c r="L114" s="125"/>
+      <c r="C114" s="160"/>
+      <c r="D114" s="160"/>
+      <c r="E114" s="160"/>
+      <c r="F114" s="160"/>
+      <c r="G114" s="160"/>
+      <c r="H114" s="160"/>
+      <c r="I114" s="160"/>
+      <c r="J114" s="160"/>
+      <c r="K114" s="160"/>
+      <c r="L114" s="160"/>
       <c r="M114" s="81"/>
     </row>
     <row r="115" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="60"/>
       <c r="B115" s="76"/>
-      <c r="C115" s="125"/>
-      <c r="D115" s="125"/>
-      <c r="E115" s="125"/>
-      <c r="F115" s="125"/>
-      <c r="G115" s="125"/>
-      <c r="H115" s="125"/>
-      <c r="I115" s="125"/>
-      <c r="J115" s="125"/>
-      <c r="K115" s="125"/>
-      <c r="L115" s="125"/>
+      <c r="C115" s="160"/>
+      <c r="D115" s="160"/>
+      <c r="E115" s="160"/>
+      <c r="F115" s="160"/>
+      <c r="G115" s="160"/>
+      <c r="H115" s="160"/>
+      <c r="I115" s="160"/>
+      <c r="J115" s="160"/>
+      <c r="K115" s="160"/>
+      <c r="L115" s="160"/>
       <c r="M115" s="81"/>
     </row>
     <row r="116" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="60"/>
       <c r="B116" s="75"/>
-      <c r="C116" s="125"/>
-      <c r="D116" s="125"/>
-      <c r="E116" s="125"/>
-      <c r="F116" s="125"/>
-      <c r="G116" s="125"/>
-      <c r="H116" s="125"/>
-      <c r="I116" s="125"/>
-      <c r="J116" s="125"/>
-      <c r="K116" s="125"/>
-      <c r="L116" s="125"/>
+      <c r="C116" s="160"/>
+      <c r="D116" s="160"/>
+      <c r="E116" s="160"/>
+      <c r="F116" s="160"/>
+      <c r="G116" s="160"/>
+      <c r="H116" s="160"/>
+      <c r="I116" s="160"/>
+      <c r="J116" s="160"/>
+      <c r="K116" s="160"/>
+      <c r="L116" s="160"/>
       <c r="M116" s="85"/>
     </row>
     <row r="117" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="60"/>
       <c r="B117" s="75"/>
-      <c r="C117" s="125"/>
-      <c r="D117" s="125"/>
-      <c r="E117" s="125"/>
-      <c r="F117" s="125"/>
-      <c r="G117" s="125"/>
-      <c r="H117" s="125"/>
-      <c r="I117" s="125"/>
-      <c r="J117" s="125"/>
-      <c r="K117" s="125"/>
-      <c r="L117" s="125"/>
+      <c r="C117" s="160"/>
+      <c r="D117" s="160"/>
+      <c r="E117" s="160"/>
+      <c r="F117" s="160"/>
+      <c r="G117" s="160"/>
+      <c r="H117" s="160"/>
+      <c r="I117" s="160"/>
+      <c r="J117" s="160"/>
+      <c r="K117" s="160"/>
+      <c r="L117" s="160"/>
       <c r="M117" s="85"/>
     </row>
     <row r="118" spans="1:14" s="23" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -32849,12 +32849,12 @@
       <c r="C124" s="46"/>
       <c r="D124" s="32"/>
       <c r="E124" s="32"/>
-      <c r="F124" s="163" t="s">
+      <c r="F124" s="111" t="s">
         <v>152</v>
       </c>
-      <c r="G124" s="163"/>
-      <c r="H124" s="163"/>
-      <c r="I124" s="163"/>
+      <c r="G124" s="111"/>
+      <c r="H124" s="111"/>
+      <c r="I124" s="111"/>
       <c r="J124"/>
       <c r="K124"/>
       <c r="L124"/>
@@ -33489,6 +33489,87 @@
     </row>
   </sheetData>
   <mergeCells count="97">
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="C74:D75"/>
+    <mergeCell ref="H74:I75"/>
+    <mergeCell ref="J74:J75"/>
+    <mergeCell ref="C72:E73"/>
+    <mergeCell ref="H72:J73"/>
+    <mergeCell ref="C112:L117"/>
+    <mergeCell ref="G28:H29"/>
+    <mergeCell ref="I28:J29"/>
+    <mergeCell ref="K28:L29"/>
+    <mergeCell ref="C100:D101"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="H98:I99"/>
+    <mergeCell ref="C98:E99"/>
+    <mergeCell ref="H100:H101"/>
+    <mergeCell ref="I100:I101"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="C39:H41"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="C43:H43"/>
+    <mergeCell ref="C62:D64"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="H61:J62"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="C94:E94"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C86:F86"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C87:D88"/>
+    <mergeCell ref="E87:E88"/>
+    <mergeCell ref="F87:F88"/>
+    <mergeCell ref="C28:D30"/>
+    <mergeCell ref="E28:F29"/>
+    <mergeCell ref="E1:K5"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="C11:L12"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
     <mergeCell ref="F124:I124"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="C80:D80"/>
@@ -33505,87 +33586,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C25:L27"/>
-    <mergeCell ref="C28:D30"/>
-    <mergeCell ref="E28:F29"/>
-    <mergeCell ref="E1:K5"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="C11:L12"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="C94:E94"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C86:F86"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C87:D88"/>
-    <mergeCell ref="E87:E88"/>
-    <mergeCell ref="F87:F88"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="C39:H41"/>
-    <mergeCell ref="C42:H42"/>
-    <mergeCell ref="C43:H43"/>
-    <mergeCell ref="C62:D64"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="H61:J62"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C112:L117"/>
-    <mergeCell ref="G28:H29"/>
-    <mergeCell ref="I28:J29"/>
-    <mergeCell ref="K28:L29"/>
-    <mergeCell ref="C100:D101"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="H98:I99"/>
-    <mergeCell ref="C98:E99"/>
-    <mergeCell ref="H100:H101"/>
-    <mergeCell ref="I100:I101"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="C74:D75"/>
-    <mergeCell ref="H74:I75"/>
-    <mergeCell ref="J74:J75"/>
-    <mergeCell ref="C72:E73"/>
-    <mergeCell ref="H72:J73"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>